<commit_message>
update ppix and code still not yet
</commit_message>
<xml_diff>
--- a/documents/Facebook Page Insight - BI Dashboard Metrics.xlsx
+++ b/documents/Facebook Page Insight - BI Dashboard Metrics.xlsx
@@ -334,7 +334,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="279">
   <si>
     <t>YÊU CẦU THIẾT KẾ TRANG FANPAGE TRÊN NỀN TẢNG POWER BI</t>
   </si>
@@ -1328,6 +1328,9 @@
   </si>
   <si>
     <t>post_consumptions_by_type</t>
+  </si>
+  <si>
+    <t>Thiếu công thức ER</t>
   </si>
 </sst>
 </file>
@@ -2578,6 +2581,147 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2621,147 +2765,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3738,8 +3741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3758,19 +3761,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="192" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
-      <c r="I1" s="145"/>
-      <c r="J1" s="145"/>
-      <c r="K1" s="145"/>
+      <c r="B1" s="192"/>
+      <c r="C1" s="192"/>
+      <c r="D1" s="192"/>
+      <c r="E1" s="192"/>
+      <c r="F1" s="192"/>
+      <c r="G1" s="192"/>
+      <c r="H1" s="192"/>
+      <c r="I1" s="192"/>
+      <c r="J1" s="192"/>
+      <c r="K1" s="192"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -3778,21 +3781,21 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="141" t="s">
+      <c r="A3" s="188" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="143"/>
-      <c r="C3" s="144"/>
-      <c r="D3" s="141" t="s">
+      <c r="B3" s="190"/>
+      <c r="C3" s="191"/>
+      <c r="D3" s="188" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="142"/>
-      <c r="F3" s="142"/>
-      <c r="G3" s="142"/>
-      <c r="H3" s="143"/>
-      <c r="I3" s="143"/>
-      <c r="J3" s="144"/>
-      <c r="K3" s="146" t="s">
+      <c r="E3" s="189"/>
+      <c r="F3" s="189"/>
+      <c r="G3" s="189"/>
+      <c r="H3" s="190"/>
+      <c r="I3" s="190"/>
+      <c r="J3" s="191"/>
+      <c r="K3" s="193" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3827,7 +3830,7 @@
       <c r="J4" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="147"/>
+      <c r="K4" s="194"/>
     </row>
     <row r="5" spans="1:11" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="64" t="s">
@@ -3852,10 +3855,10 @@
       <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="138" t="s">
+      <c r="B6" s="185" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="135" t="s">
+      <c r="C6" s="182" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="95" t="s">
@@ -3873,10 +3876,10 @@
       <c r="H6" s="33" t="s">
         <v>247</v>
       </c>
-      <c r="I6" s="150" t="s">
+      <c r="I6" s="168" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="135" t="s">
+      <c r="J6" s="182" t="s">
         <v>32</v>
       </c>
       <c r="K6" s="70"/>
@@ -3885,8 +3888,8 @@
       <c r="A7" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="139"/>
-      <c r="C7" s="136"/>
+      <c r="B7" s="186"/>
+      <c r="C7" s="183"/>
       <c r="D7" s="95" t="s">
         <v>57</v>
       </c>
@@ -3902,16 +3905,18 @@
       <c r="H7" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="I7" s="151"/>
-      <c r="J7" s="136"/>
-      <c r="K7" s="71"/>
+      <c r="I7" s="169"/>
+      <c r="J7" s="183"/>
+      <c r="K7" s="71" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="139"/>
-      <c r="C8" s="136"/>
+      <c r="B8" s="186"/>
+      <c r="C8" s="183"/>
       <c r="D8" s="95" t="s">
         <v>67</v>
       </c>
@@ -3927,16 +3932,16 @@
       <c r="H8" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="151"/>
-      <c r="J8" s="136"/>
+      <c r="I8" s="169"/>
+      <c r="J8" s="183"/>
       <c r="K8" s="71"/>
     </row>
     <row r="9" spans="1:11" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="139"/>
-      <c r="C9" s="136"/>
+      <c r="B9" s="186"/>
+      <c r="C9" s="183"/>
       <c r="D9" s="95" t="s">
         <v>46</v>
       </c>
@@ -3952,16 +3957,16 @@
       <c r="H9" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="I9" s="151"/>
-      <c r="J9" s="136"/>
+      <c r="I9" s="169"/>
+      <c r="J9" s="183"/>
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="148" t="s">
+      <c r="A10" s="195" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="139"/>
-      <c r="C10" s="136"/>
+      <c r="B10" s="186"/>
+      <c r="C10" s="183"/>
       <c r="D10" s="96" t="s">
         <v>120</v>
       </c>
@@ -3974,17 +3979,17 @@
       <c r="G10" s="93" t="s">
         <v>79</v>
       </c>
-      <c r="H10" s="153" t="s">
+      <c r="H10" s="148" t="s">
         <v>124</v>
       </c>
-      <c r="I10" s="151"/>
-      <c r="J10" s="136"/>
+      <c r="I10" s="169"/>
+      <c r="J10" s="183"/>
       <c r="K10" s="71"/>
     </row>
     <row r="11" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="149"/>
-      <c r="B11" s="139"/>
-      <c r="C11" s="136"/>
+      <c r="A11" s="196"/>
+      <c r="B11" s="186"/>
+      <c r="C11" s="183"/>
       <c r="D11" s="97" t="s">
         <v>118</v>
       </c>
@@ -3997,17 +4002,17 @@
       <c r="G11" s="94" t="s">
         <v>79</v>
       </c>
-      <c r="H11" s="154"/>
-      <c r="I11" s="151"/>
-      <c r="J11" s="136"/>
+      <c r="H11" s="149"/>
+      <c r="I11" s="169"/>
+      <c r="J11" s="183"/>
       <c r="K11" s="71"/>
     </row>
     <row r="12" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="139"/>
-      <c r="C12" s="136"/>
+      <c r="B12" s="186"/>
+      <c r="C12" s="183"/>
       <c r="D12" s="98" t="s">
         <v>72</v>
       </c>
@@ -4023,16 +4028,16 @@
       <c r="H12" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="I12" s="151"/>
-      <c r="J12" s="136"/>
+      <c r="I12" s="169"/>
+      <c r="J12" s="183"/>
       <c r="K12" s="71"/>
     </row>
     <row r="13" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="72" t="s">
         <v>76</v>
       </c>
-      <c r="B13" s="140"/>
-      <c r="C13" s="137"/>
+      <c r="B13" s="187"/>
+      <c r="C13" s="184"/>
       <c r="D13" s="99" t="s">
         <v>46</v>
       </c>
@@ -4046,8 +4051,8 @@
       <c r="H13" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="I13" s="152"/>
-      <c r="J13" s="137"/>
+      <c r="I13" s="170"/>
+      <c r="J13" s="184"/>
       <c r="K13" s="75"/>
     </row>
     <row r="14" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -4073,10 +4078,10 @@
       <c r="A15" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="155" t="s">
+      <c r="B15" s="174" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="157" t="s">
+      <c r="C15" s="163" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="95" t="str">
@@ -4099,10 +4104,10 @@
         <f>H6</f>
         <v>Giá trị của ngày cuối cùng tại thời điểm lấy dữ liệu</v>
       </c>
-      <c r="I15" s="150" t="s">
+      <c r="I15" s="168" t="s">
         <v>49</v>
       </c>
-      <c r="J15" s="157" t="s">
+      <c r="J15" s="163" t="s">
         <v>32</v>
       </c>
       <c r="K15" s="52"/>
@@ -4111,8 +4116,8 @@
       <c r="A16" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="155"/>
-      <c r="C16" s="157"/>
+      <c r="B16" s="174"/>
+      <c r="C16" s="163"/>
       <c r="D16" s="98" t="s">
         <v>82</v>
       </c>
@@ -4128,8 +4133,8 @@
       <c r="H16" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="I16" s="151"/>
-      <c r="J16" s="157"/>
+      <c r="I16" s="169"/>
+      <c r="J16" s="163"/>
       <c r="K16" s="53" t="s">
         <v>111</v>
       </c>
@@ -4138,8 +4143,8 @@
       <c r="A17" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="B17" s="155"/>
-      <c r="C17" s="157"/>
+      <c r="B17" s="174"/>
+      <c r="C17" s="163"/>
       <c r="D17" s="98" t="s">
         <v>110</v>
       </c>
@@ -4155,8 +4160,8 @@
       <c r="H17" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="I17" s="151"/>
-      <c r="J17" s="157"/>
+      <c r="I17" s="169"/>
+      <c r="J17" s="163"/>
       <c r="K17" s="54" t="s">
         <v>112</v>
       </c>
@@ -4165,8 +4170,8 @@
       <c r="A18" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="156"/>
-      <c r="C18" s="158"/>
+      <c r="B18" s="175"/>
+      <c r="C18" s="164"/>
       <c r="D18" s="101" t="s">
         <v>84</v>
       </c>
@@ -4182,8 +4187,8 @@
       <c r="H18" s="33" t="s">
         <v>247</v>
       </c>
-      <c r="I18" s="152"/>
-      <c r="J18" s="158"/>
+      <c r="I18" s="170"/>
+      <c r="J18" s="164"/>
       <c r="K18" s="59" t="s">
         <v>228</v>
       </c>
@@ -4211,10 +4216,10 @@
       <c r="A20" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="159" t="s">
+      <c r="B20" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="161" t="s">
+      <c r="C20" s="152" t="s">
         <v>32</v>
       </c>
       <c r="D20" s="96" t="s">
@@ -4232,13 +4237,13 @@
       <c r="H20" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="I20" s="172" t="s">
+      <c r="I20" s="146" t="s">
         <v>50</v>
       </c>
-      <c r="J20" s="161" t="s">
+      <c r="J20" s="152" t="s">
         <v>32</v>
       </c>
-      <c r="K20" s="178" t="s">
+      <c r="K20" s="137" t="s">
         <v>112</v>
       </c>
     </row>
@@ -4246,8 +4251,8 @@
       <c r="A21" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="160"/>
-      <c r="C21" s="162"/>
+      <c r="B21" s="177"/>
+      <c r="C21" s="154"/>
       <c r="D21" s="100" t="s">
         <v>117</v>
       </c>
@@ -4263,9 +4268,9 @@
       <c r="H21" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="I21" s="173"/>
-      <c r="J21" s="162"/>
-      <c r="K21" s="179"/>
+      <c r="I21" s="171"/>
+      <c r="J21" s="154"/>
+      <c r="K21" s="138"/>
     </row>
     <row r="22" spans="1:23" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="76" t="s">
@@ -4287,13 +4292,13 @@
       <c r="K22" s="80"/>
     </row>
     <row r="23" spans="1:23" s="85" customFormat="1" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="181" t="s">
+      <c r="A23" s="142" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="183" t="s">
+      <c r="B23" s="144" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="161" t="s">
+      <c r="C23" s="152" t="s">
         <v>32</v>
       </c>
       <c r="D23" s="96" t="s">
@@ -4308,21 +4313,21 @@
       <c r="G23" s="93" t="s">
         <v>79</v>
       </c>
-      <c r="H23" s="153" t="s">
+      <c r="H23" s="148" t="s">
         <v>127</v>
       </c>
-      <c r="I23" s="172" t="s">
+      <c r="I23" s="146" t="s">
         <v>50</v>
       </c>
-      <c r="J23" s="169" t="s">
+      <c r="J23" s="165" t="s">
         <v>32</v>
       </c>
-      <c r="K23" s="177"/>
+      <c r="K23" s="136"/>
     </row>
     <row r="24" spans="1:23" s="85" customFormat="1" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="182"/>
-      <c r="B24" s="184"/>
-      <c r="C24" s="188"/>
+      <c r="A24" s="143"/>
+      <c r="B24" s="145"/>
+      <c r="C24" s="153"/>
       <c r="D24" s="97" t="s">
         <v>118</v>
       </c>
@@ -4335,39 +4340,39 @@
       <c r="G24" s="94" t="s">
         <v>79</v>
       </c>
-      <c r="H24" s="154"/>
-      <c r="I24" s="185"/>
-      <c r="J24" s="170"/>
-      <c r="K24" s="177"/>
+      <c r="H24" s="149"/>
+      <c r="I24" s="147"/>
+      <c r="J24" s="166"/>
+      <c r="K24" s="136"/>
     </row>
     <row r="25" spans="1:23" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="118" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="183" t="s">
+      <c r="B25" s="144" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="188"/>
-      <c r="D25" s="166" t="s">
+      <c r="C25" s="153"/>
+      <c r="D25" s="179" t="s">
         <v>129</v>
       </c>
       <c r="E25" s="102" t="s">
         <v>130</v>
       </c>
-      <c r="F25" s="163" t="s">
+      <c r="F25" s="139" t="s">
         <v>128</v>
       </c>
-      <c r="G25" s="189" t="s">
+      <c r="G25" s="155" t="s">
         <v>46</v>
       </c>
       <c r="H25" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="I25" s="172" t="s">
+      <c r="I25" s="146" t="s">
         <v>48</v>
       </c>
-      <c r="J25" s="170"/>
-      <c r="K25" s="176" t="s">
+      <c r="J25" s="166"/>
+      <c r="K25" s="135" t="s">
         <v>239</v>
       </c>
     </row>
@@ -4375,62 +4380,62 @@
       <c r="A26" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="186"/>
-      <c r="C26" s="188"/>
-      <c r="D26" s="167"/>
+      <c r="B26" s="150"/>
+      <c r="C26" s="153"/>
+      <c r="D26" s="180"/>
       <c r="E26" s="102" t="s">
         <v>131</v>
       </c>
-      <c r="F26" s="164"/>
-      <c r="G26" s="190"/>
+      <c r="F26" s="140"/>
+      <c r="G26" s="156"/>
       <c r="H26" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="I26" s="174"/>
-      <c r="J26" s="170"/>
-      <c r="K26" s="177"/>
+      <c r="I26" s="172"/>
+      <c r="J26" s="166"/>
+      <c r="K26" s="136"/>
     </row>
     <row r="27" spans="1:23" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="118" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="186"/>
-      <c r="C27" s="188"/>
-      <c r="D27" s="168"/>
+      <c r="B27" s="150"/>
+      <c r="C27" s="153"/>
+      <c r="D27" s="181"/>
       <c r="E27" s="102" t="s">
         <v>132</v>
       </c>
-      <c r="F27" s="165"/>
-      <c r="G27" s="191"/>
+      <c r="F27" s="178"/>
+      <c r="G27" s="157"/>
       <c r="H27" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="I27" s="174"/>
-      <c r="J27" s="170"/>
-      <c r="K27" s="177"/>
+      <c r="I27" s="172"/>
+      <c r="J27" s="166"/>
+      <c r="K27" s="136"/>
     </row>
     <row r="28" spans="1:23" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="186"/>
-      <c r="C28" s="188"/>
-      <c r="D28" s="193"/>
+      <c r="B28" s="150"/>
+      <c r="C28" s="153"/>
+      <c r="D28" s="159"/>
       <c r="E28" s="28" t="s">
         <v>235</v>
       </c>
-      <c r="F28" s="163" t="s">
+      <c r="F28" s="139" t="s">
         <v>229</v>
       </c>
-      <c r="G28" s="189" t="s">
+      <c r="G28" s="155" t="s">
         <v>46</v>
       </c>
       <c r="H28" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="I28" s="174"/>
-      <c r="J28" s="170"/>
-      <c r="K28" s="176" t="s">
+      <c r="I28" s="172"/>
+      <c r="J28" s="166"/>
+      <c r="K28" s="135" t="s">
         <v>240</v>
       </c>
     </row>
@@ -4438,58 +4443,58 @@
       <c r="A29" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="186"/>
-      <c r="C29" s="188"/>
-      <c r="D29" s="194"/>
+      <c r="B29" s="150"/>
+      <c r="C29" s="153"/>
+      <c r="D29" s="160"/>
       <c r="E29" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="F29" s="164"/>
-      <c r="G29" s="190"/>
+      <c r="F29" s="140"/>
+      <c r="G29" s="156"/>
       <c r="H29" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="I29" s="174"/>
-      <c r="J29" s="170"/>
-      <c r="K29" s="177"/>
+      <c r="I29" s="172"/>
+      <c r="J29" s="166"/>
+      <c r="K29" s="136"/>
     </row>
     <row r="30" spans="1:23" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="118" t="s">
         <v>234</v>
       </c>
-      <c r="B30" s="186"/>
-      <c r="C30" s="188"/>
-      <c r="D30" s="194"/>
+      <c r="B30" s="150"/>
+      <c r="C30" s="153"/>
+      <c r="D30" s="160"/>
       <c r="E30" s="28" t="s">
         <v>237</v>
       </c>
-      <c r="F30" s="164"/>
-      <c r="G30" s="190"/>
+      <c r="F30" s="140"/>
+      <c r="G30" s="156"/>
       <c r="H30" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="I30" s="174"/>
-      <c r="J30" s="170"/>
-      <c r="K30" s="177"/>
+      <c r="I30" s="172"/>
+      <c r="J30" s="166"/>
+      <c r="K30" s="136"/>
     </row>
     <row r="31" spans="1:23" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="119" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="187"/>
-      <c r="C31" s="162"/>
-      <c r="D31" s="195"/>
+      <c r="B31" s="151"/>
+      <c r="C31" s="154"/>
+      <c r="D31" s="161"/>
       <c r="E31" s="29" t="s">
         <v>238</v>
       </c>
-      <c r="F31" s="180"/>
-      <c r="G31" s="192"/>
+      <c r="F31" s="141"/>
+      <c r="G31" s="158"/>
       <c r="H31" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="I31" s="175"/>
-      <c r="J31" s="171"/>
-      <c r="K31" s="196"/>
+      <c r="I31" s="173"/>
+      <c r="J31" s="167"/>
+      <c r="K31" s="162"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="M32" s="1"/>
@@ -4818,6 +4823,28 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="C6:C13"/>
+    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="D3:J3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="J6:J13"/>
+    <mergeCell ref="I6:I13"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="J15:J18"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="J23:J31"/>
+    <mergeCell ref="I15:I18"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="I25:I31"/>
     <mergeCell ref="K25:K27"/>
     <mergeCell ref="K20:K21"/>
     <mergeCell ref="F28:F31"/>
@@ -4832,28 +4859,6 @@
     <mergeCell ref="G28:G31"/>
     <mergeCell ref="D28:D31"/>
     <mergeCell ref="K28:K31"/>
-    <mergeCell ref="J15:J18"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="J23:J31"/>
-    <mergeCell ref="I15:I18"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="I25:I31"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="C6:C13"/>
-    <mergeCell ref="B6:B13"/>
-    <mergeCell ref="D3:J3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="J6:J13"/>
-    <mergeCell ref="I6:I13"/>
-    <mergeCell ref="H10:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4867,7 +4872,7 @@
   <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15:M15"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
delete bản cũ và update
</commit_message>
<xml_diff>
--- a/documents/Facebook Page Insight - BI Dashboard Metrics.xlsx
+++ b/documents/Facebook Page Insight - BI Dashboard Metrics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="516" windowWidth="23040" windowHeight="8676"/>
+    <workbookView xWindow="0" yWindow="516" windowWidth="23040" windowHeight="8676" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="1. Yêu cầu thiết kế" sheetId="1" r:id="rId1"/>
@@ -334,7 +334,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="281">
   <si>
     <t>YÊU CẦU THIẾT KẾ TRANG FANPAGE TRÊN NỀN TẢNG POWER BI</t>
   </si>
@@ -1334,6 +1334,9 @@
   </si>
   <si>
     <t>Giá trị của ngày cuối cùng trong 1 Tháng hoặc 1 Năm.</t>
+  </si>
+  <si>
+    <t>((d10+d11)/d7)*100</t>
   </si>
 </sst>
 </file>
@@ -2587,6 +2590,150 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2632,147 +2779,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2853,9 +2859,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3750,8 +3753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:H31"/>
+    <sheetView zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3770,19 +3773,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="194" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="146"/>
-      <c r="J1" s="146"/>
-      <c r="K1" s="146"/>
+      <c r="B1" s="194"/>
+      <c r="C1" s="194"/>
+      <c r="D1" s="194"/>
+      <c r="E1" s="194"/>
+      <c r="F1" s="194"/>
+      <c r="G1" s="194"/>
+      <c r="H1" s="194"/>
+      <c r="I1" s="194"/>
+      <c r="J1" s="194"/>
+      <c r="K1" s="194"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -3790,21 +3793,21 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="142" t="s">
+      <c r="A3" s="190" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="144"/>
-      <c r="C3" s="145"/>
-      <c r="D3" s="142" t="s">
+      <c r="B3" s="192"/>
+      <c r="C3" s="193"/>
+      <c r="D3" s="190" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="143"/>
-      <c r="F3" s="143"/>
-      <c r="G3" s="143"/>
-      <c r="H3" s="144"/>
-      <c r="I3" s="144"/>
-      <c r="J3" s="145"/>
-      <c r="K3" s="147" t="s">
+      <c r="E3" s="191"/>
+      <c r="F3" s="191"/>
+      <c r="G3" s="191"/>
+      <c r="H3" s="192"/>
+      <c r="I3" s="192"/>
+      <c r="J3" s="193"/>
+      <c r="K3" s="195" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3839,7 +3842,7 @@
       <c r="J4" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="148"/>
+      <c r="K4" s="196"/>
     </row>
     <row r="5" spans="1:11" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="64" t="s">
@@ -3864,10 +3867,10 @@
       <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="139" t="s">
+      <c r="B6" s="187" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="136" t="s">
+      <c r="C6" s="184" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="95" t="s">
@@ -3885,10 +3888,10 @@
       <c r="H6" s="33" t="s">
         <v>279</v>
       </c>
-      <c r="I6" s="151" t="s">
+      <c r="I6" s="170" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="136" t="s">
+      <c r="J6" s="184" t="s">
         <v>32</v>
       </c>
       <c r="K6" s="70"/>
@@ -3897,8 +3900,8 @@
       <c r="A7" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="140"/>
-      <c r="C7" s="137"/>
+      <c r="B7" s="188"/>
+      <c r="C7" s="185"/>
       <c r="D7" s="95" t="s">
         <v>57</v>
       </c>
@@ -3914,8 +3917,8 @@
       <c r="H7" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="I7" s="152"/>
-      <c r="J7" s="137"/>
+      <c r="I7" s="171"/>
+      <c r="J7" s="185"/>
       <c r="K7" s="71" t="s">
         <v>277</v>
       </c>
@@ -3924,8 +3927,8 @@
       <c r="A8" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="140"/>
-      <c r="C8" s="137"/>
+      <c r="B8" s="188"/>
+      <c r="C8" s="185"/>
       <c r="D8" s="95" t="s">
         <v>67</v>
       </c>
@@ -3941,16 +3944,16 @@
       <c r="H8" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="152"/>
-      <c r="J8" s="137"/>
+      <c r="I8" s="171"/>
+      <c r="J8" s="185"/>
       <c r="K8" s="71"/>
     </row>
     <row r="9" spans="1:11" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="140"/>
-      <c r="C9" s="137"/>
+      <c r="B9" s="188"/>
+      <c r="C9" s="185"/>
       <c r="D9" s="95" t="s">
         <v>46</v>
       </c>
@@ -3966,16 +3969,16 @@
       <c r="H9" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="I9" s="152"/>
-      <c r="J9" s="137"/>
+      <c r="I9" s="171"/>
+      <c r="J9" s="185"/>
       <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="149" t="s">
+      <c r="A10" s="197" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="140"/>
-      <c r="C10" s="137"/>
+      <c r="B10" s="188"/>
+      <c r="C10" s="185"/>
       <c r="D10" s="96" t="s">
         <v>120</v>
       </c>
@@ -3988,17 +3991,17 @@
       <c r="G10" s="93" t="s">
         <v>79</v>
       </c>
-      <c r="H10" s="154" t="s">
+      <c r="H10" s="163" t="s">
         <v>124</v>
       </c>
-      <c r="I10" s="152"/>
-      <c r="J10" s="137"/>
+      <c r="I10" s="171"/>
+      <c r="J10" s="185"/>
       <c r="K10" s="71"/>
     </row>
     <row r="11" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="150"/>
-      <c r="B11" s="140"/>
-      <c r="C11" s="137"/>
+      <c r="A11" s="198"/>
+      <c r="B11" s="188"/>
+      <c r="C11" s="185"/>
       <c r="D11" s="97" t="s">
         <v>118</v>
       </c>
@@ -4011,34 +4014,34 @@
       <c r="G11" s="94" t="s">
         <v>79</v>
       </c>
-      <c r="H11" s="155"/>
-      <c r="I11" s="152"/>
-      <c r="J11" s="137"/>
+      <c r="H11" s="164"/>
+      <c r="I11" s="171"/>
+      <c r="J11" s="185"/>
       <c r="K11" s="71"/>
     </row>
     <row r="12" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="135" t="s">
         <v>278</v>
       </c>
-      <c r="B12" s="140"/>
-      <c r="C12" s="137"/>
+      <c r="B12" s="188"/>
+      <c r="C12" s="185"/>
       <c r="D12" s="97"/>
       <c r="E12" s="86"/>
       <c r="F12" s="38"/>
       <c r="G12" s="94"/>
       <c r="H12" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="I12" s="152"/>
-      <c r="J12" s="137"/>
+        <v>280</v>
+      </c>
+      <c r="I12" s="171"/>
+      <c r="J12" s="185"/>
       <c r="K12" s="71"/>
     </row>
     <row r="13" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="140"/>
-      <c r="C13" s="137"/>
+      <c r="B13" s="188"/>
+      <c r="C13" s="185"/>
       <c r="D13" s="98" t="s">
         <v>72</v>
       </c>
@@ -4054,16 +4057,16 @@
       <c r="H13" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="I13" s="152"/>
-      <c r="J13" s="137"/>
+      <c r="I13" s="171"/>
+      <c r="J13" s="185"/>
       <c r="K13" s="71"/>
     </row>
     <row r="14" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="72" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="141"/>
-      <c r="C14" s="138"/>
+      <c r="B14" s="189"/>
+      <c r="C14" s="186"/>
       <c r="D14" s="99" t="s">
         <v>46</v>
       </c>
@@ -4075,8 +4078,8 @@
       </c>
       <c r="G14" s="88"/>
       <c r="H14" s="47"/>
-      <c r="I14" s="153"/>
-      <c r="J14" s="138"/>
+      <c r="I14" s="172"/>
+      <c r="J14" s="186"/>
       <c r="K14" s="75"/>
     </row>
     <row r="15" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -4105,10 +4108,10 @@
       <c r="A16" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="156" t="s">
+      <c r="B16" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="158" t="s">
+      <c r="C16" s="165" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="95" t="str">
@@ -4130,10 +4133,10 @@
       <c r="H16" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="I16" s="151" t="s">
+      <c r="I16" s="170" t="s">
         <v>49</v>
       </c>
-      <c r="J16" s="158" t="s">
+      <c r="J16" s="165" t="s">
         <v>32</v>
       </c>
       <c r="K16" s="52"/>
@@ -4142,8 +4145,8 @@
       <c r="A17" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="156"/>
-      <c r="C17" s="158"/>
+      <c r="B17" s="176"/>
+      <c r="C17" s="165"/>
       <c r="D17" s="98" t="s">
         <v>82</v>
       </c>
@@ -4159,8 +4162,8 @@
       <c r="H17" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="I17" s="152"/>
-      <c r="J17" s="158"/>
+      <c r="I17" s="171"/>
+      <c r="J17" s="165"/>
       <c r="K17" s="53" t="s">
         <v>111</v>
       </c>
@@ -4169,8 +4172,8 @@
       <c r="A18" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="B18" s="156"/>
-      <c r="C18" s="158"/>
+      <c r="B18" s="176"/>
+      <c r="C18" s="165"/>
       <c r="D18" s="98" t="s">
         <v>110</v>
       </c>
@@ -4186,8 +4189,8 @@
       <c r="H18" s="58" t="s">
         <v>279</v>
       </c>
-      <c r="I18" s="152"/>
-      <c r="J18" s="158"/>
+      <c r="I18" s="171"/>
+      <c r="J18" s="165"/>
       <c r="K18" s="54" t="s">
         <v>112</v>
       </c>
@@ -4196,8 +4199,8 @@
       <c r="A19" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="157"/>
-      <c r="C19" s="159"/>
+      <c r="B19" s="177"/>
+      <c r="C19" s="166"/>
       <c r="D19" s="101" t="s">
         <v>84</v>
       </c>
@@ -4211,8 +4214,8 @@
         <v>46</v>
       </c>
       <c r="H19" s="78"/>
-      <c r="I19" s="153"/>
-      <c r="J19" s="159"/>
+      <c r="I19" s="172"/>
+      <c r="J19" s="166"/>
       <c r="K19" s="59" t="s">
         <v>228</v>
       </c>
@@ -4242,10 +4245,10 @@
       <c r="A21" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="160" t="s">
+      <c r="B21" s="178" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="162" t="s">
+      <c r="C21" s="152" t="s">
         <v>32</v>
       </c>
       <c r="D21" s="96" t="s">
@@ -4263,13 +4266,13 @@
       <c r="H21" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="I21" s="173" t="s">
+      <c r="I21" s="148" t="s">
         <v>50</v>
       </c>
-      <c r="J21" s="162" t="s">
+      <c r="J21" s="152" t="s">
         <v>32</v>
       </c>
-      <c r="K21" s="179" t="s">
+      <c r="K21" s="139" t="s">
         <v>112</v>
       </c>
     </row>
@@ -4277,8 +4280,8 @@
       <c r="A22" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="161"/>
-      <c r="C22" s="163"/>
+      <c r="B22" s="179"/>
+      <c r="C22" s="154"/>
       <c r="D22" s="100" t="s">
         <v>117</v>
       </c>
@@ -4292,9 +4295,9 @@
         <v>79</v>
       </c>
       <c r="H22" s="78"/>
-      <c r="I22" s="174"/>
-      <c r="J22" s="163"/>
-      <c r="K22" s="180"/>
+      <c r="I22" s="173"/>
+      <c r="J22" s="154"/>
+      <c r="K22" s="140"/>
     </row>
     <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="76" t="s">
@@ -4310,7 +4313,7 @@
       <c r="E23" s="77"/>
       <c r="F23" s="77"/>
       <c r="G23" s="89"/>
-      <c r="H23" s="154" t="s">
+      <c r="H23" s="163" t="s">
         <v>127</v>
       </c>
       <c r="I23" s="78"/>
@@ -4318,13 +4321,13 @@
       <c r="K23" s="80"/>
     </row>
     <row r="24" spans="1:11" s="85" customFormat="1" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="182" t="s">
+      <c r="A24" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="184" t="s">
+      <c r="B24" s="146" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="162" t="s">
+      <c r="C24" s="152" t="s">
         <v>32</v>
       </c>
       <c r="D24" s="96" t="s">
@@ -4339,19 +4342,19 @@
       <c r="G24" s="93" t="s">
         <v>79</v>
       </c>
-      <c r="H24" s="155"/>
-      <c r="I24" s="173" t="s">
+      <c r="H24" s="164"/>
+      <c r="I24" s="148" t="s">
         <v>50</v>
       </c>
-      <c r="J24" s="170" t="s">
+      <c r="J24" s="167" t="s">
         <v>32</v>
       </c>
-      <c r="K24" s="178"/>
+      <c r="K24" s="138"/>
     </row>
     <row r="25" spans="1:11" s="85" customFormat="1" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="183"/>
-      <c r="B25" s="185"/>
-      <c r="C25" s="189"/>
+      <c r="A25" s="145"/>
+      <c r="B25" s="147"/>
+      <c r="C25" s="153"/>
       <c r="D25" s="97" t="s">
         <v>118</v>
       </c>
@@ -4367,38 +4370,38 @@
       <c r="H25" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="I25" s="186"/>
-      <c r="J25" s="171"/>
-      <c r="K25" s="178"/>
+      <c r="I25" s="149"/>
+      <c r="J25" s="168"/>
+      <c r="K25" s="138"/>
     </row>
     <row r="26" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="118" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="184" t="s">
+      <c r="B26" s="146" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="189"/>
-      <c r="D26" s="167" t="s">
+      <c r="C26" s="153"/>
+      <c r="D26" s="181" t="s">
         <v>129</v>
       </c>
       <c r="E26" s="102" t="s">
         <v>130</v>
       </c>
-      <c r="F26" s="164" t="s">
+      <c r="F26" s="141" t="s">
         <v>128</v>
       </c>
-      <c r="G26" s="190" t="s">
+      <c r="G26" s="155" t="s">
         <v>46</v>
       </c>
       <c r="H26" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="I26" s="173" t="s">
+      <c r="I26" s="148" t="s">
         <v>48</v>
       </c>
-      <c r="J26" s="171"/>
-      <c r="K26" s="177" t="s">
+      <c r="J26" s="168"/>
+      <c r="K26" s="137" t="s">
         <v>239</v>
       </c>
     </row>
@@ -4406,62 +4409,62 @@
       <c r="A27" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="187"/>
-      <c r="C27" s="189"/>
-      <c r="D27" s="168"/>
+      <c r="B27" s="150"/>
+      <c r="C27" s="153"/>
+      <c r="D27" s="182"/>
       <c r="E27" s="102" t="s">
         <v>131</v>
       </c>
-      <c r="F27" s="165"/>
-      <c r="G27" s="191"/>
+      <c r="F27" s="142"/>
+      <c r="G27" s="156"/>
       <c r="H27" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="I27" s="175"/>
-      <c r="J27" s="171"/>
-      <c r="K27" s="178"/>
+      <c r="I27" s="174"/>
+      <c r="J27" s="168"/>
+      <c r="K27" s="138"/>
     </row>
     <row r="28" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="118" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="187"/>
-      <c r="C28" s="189"/>
-      <c r="D28" s="169"/>
+      <c r="B28" s="150"/>
+      <c r="C28" s="153"/>
+      <c r="D28" s="183"/>
       <c r="E28" s="102" t="s">
         <v>132</v>
       </c>
-      <c r="F28" s="166"/>
-      <c r="G28" s="192"/>
+      <c r="F28" s="180"/>
+      <c r="G28" s="157"/>
       <c r="H28" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="I28" s="175"/>
-      <c r="J28" s="171"/>
-      <c r="K28" s="178"/>
+      <c r="I28" s="174"/>
+      <c r="J28" s="168"/>
+      <c r="K28" s="138"/>
     </row>
     <row r="29" spans="1:11" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="187"/>
-      <c r="C29" s="189"/>
-      <c r="D29" s="194"/>
+      <c r="B29" s="150"/>
+      <c r="C29" s="153"/>
+      <c r="D29" s="159"/>
       <c r="E29" s="28" t="s">
         <v>235</v>
       </c>
-      <c r="F29" s="164" t="s">
+      <c r="F29" s="141" t="s">
         <v>229</v>
       </c>
-      <c r="G29" s="190" t="s">
+      <c r="G29" s="155" t="s">
         <v>46</v>
       </c>
       <c r="H29" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="I29" s="175"/>
-      <c r="J29" s="171"/>
-      <c r="K29" s="177" t="s">
+      <c r="I29" s="174"/>
+      <c r="J29" s="168"/>
+      <c r="K29" s="137" t="s">
         <v>240</v>
       </c>
     </row>
@@ -4469,58 +4472,58 @@
       <c r="A30" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="187"/>
-      <c r="C30" s="189"/>
-      <c r="D30" s="195"/>
+      <c r="B30" s="150"/>
+      <c r="C30" s="153"/>
+      <c r="D30" s="160"/>
       <c r="E30" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="F30" s="165"/>
-      <c r="G30" s="191"/>
+      <c r="F30" s="142"/>
+      <c r="G30" s="156"/>
       <c r="H30" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="I30" s="175"/>
-      <c r="J30" s="171"/>
-      <c r="K30" s="178"/>
+      <c r="I30" s="174"/>
+      <c r="J30" s="168"/>
+      <c r="K30" s="138"/>
     </row>
     <row r="31" spans="1:11" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="118" t="s">
         <v>234</v>
       </c>
-      <c r="B31" s="187"/>
-      <c r="C31" s="189"/>
-      <c r="D31" s="195"/>
+      <c r="B31" s="150"/>
+      <c r="C31" s="153"/>
+      <c r="D31" s="160"/>
       <c r="E31" s="28" t="s">
         <v>237</v>
       </c>
-      <c r="F31" s="165"/>
-      <c r="G31" s="191"/>
+      <c r="F31" s="142"/>
+      <c r="G31" s="156"/>
       <c r="H31" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="I31" s="175"/>
-      <c r="J31" s="171"/>
-      <c r="K31" s="178"/>
+      <c r="I31" s="174"/>
+      <c r="J31" s="168"/>
+      <c r="K31" s="138"/>
     </row>
     <row r="32" spans="1:11" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="119" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="188"/>
-      <c r="C32" s="163"/>
-      <c r="D32" s="196"/>
+      <c r="B32" s="151"/>
+      <c r="C32" s="154"/>
+      <c r="D32" s="161"/>
       <c r="E32" s="29" t="s">
         <v>238</v>
       </c>
-      <c r="F32" s="181"/>
-      <c r="G32" s="193"/>
+      <c r="F32" s="143"/>
+      <c r="G32" s="158"/>
       <c r="H32" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="I32" s="176"/>
-      <c r="J32" s="172"/>
-      <c r="K32" s="197"/>
+      <c r="I32" s="175"/>
+      <c r="J32" s="169"/>
+      <c r="K32" s="162"/>
     </row>
     <row r="33" spans="13:23" x14ac:dyDescent="0.3">
       <c r="M33" s="1"/>
@@ -4849,6 +4852,28 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="C6:C14"/>
+    <mergeCell ref="B6:B14"/>
+    <mergeCell ref="D3:J3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="J6:J14"/>
+    <mergeCell ref="I6:I14"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="J24:J32"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="I26:I32"/>
     <mergeCell ref="K26:K28"/>
     <mergeCell ref="K21:K22"/>
     <mergeCell ref="F29:F32"/>
@@ -4863,28 +4888,6 @@
     <mergeCell ref="D29:D32"/>
     <mergeCell ref="K29:K32"/>
     <mergeCell ref="H23:H24"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="J24:J32"/>
-    <mergeCell ref="I16:I19"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="I26:I32"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="C6:C14"/>
-    <mergeCell ref="B6:B14"/>
-    <mergeCell ref="D3:J3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="J6:J14"/>
-    <mergeCell ref="I6:I14"/>
-    <mergeCell ref="H10:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4932,23 +4935,23 @@
     </row>
     <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A5" s="200" t="s">
+      <c r="A5" s="201" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="201"/>
-      <c r="C5" s="202"/>
+      <c r="B5" s="202"/>
+      <c r="C5" s="203"/>
       <c r="D5" s="14"/>
-      <c r="E5" s="200" t="s">
+      <c r="E5" s="201" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="201"/>
-      <c r="G5" s="201"/>
-      <c r="H5" s="201"/>
-      <c r="I5" s="201"/>
-      <c r="J5" s="201"/>
-      <c r="K5" s="201"/>
-      <c r="L5" s="201"/>
-      <c r="M5" s="202"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="202"/>
+      <c r="H5" s="202"/>
+      <c r="I5" s="202"/>
+      <c r="J5" s="202"/>
+      <c r="K5" s="202"/>
+      <c r="L5" s="202"/>
+      <c r="M5" s="203"/>
     </row>
     <row r="6" spans="1:13" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
@@ -4960,21 +4963,21 @@
       <c r="C6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="207" t="s">
+      <c r="E6" s="208" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="208"/>
+      <c r="F6" s="209"/>
       <c r="G6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="222" t="s">
+      <c r="H6" s="223" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="223"/>
-      <c r="J6" s="223"/>
-      <c r="K6" s="223"/>
-      <c r="L6" s="223"/>
-      <c r="M6" s="224"/>
+      <c r="I6" s="224"/>
+      <c r="J6" s="224"/>
+      <c r="K6" s="224"/>
+      <c r="L6" s="224"/>
+      <c r="M6" s="225"/>
     </row>
     <row r="7" spans="1:13" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
@@ -4986,19 +4989,19 @@
       <c r="C7" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="209" t="s">
+      <c r="E7" s="210" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="210"/>
-      <c r="G7" s="210"/>
-      <c r="H7" s="213" t="s">
+      <c r="F7" s="211"/>
+      <c r="G7" s="211"/>
+      <c r="H7" s="214" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="214"/>
-      <c r="J7" s="214"/>
-      <c r="K7" s="214"/>
-      <c r="L7" s="214"/>
-      <c r="M7" s="215"/>
+      <c r="I7" s="215"/>
+      <c r="J7" s="215"/>
+      <c r="K7" s="215"/>
+      <c r="L7" s="215"/>
+      <c r="M7" s="216"/>
     </row>
     <row r="8" spans="1:13" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
@@ -5010,15 +5013,15 @@
       <c r="C8" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="209"/>
-      <c r="F8" s="210"/>
-      <c r="G8" s="210"/>
-      <c r="H8" s="216"/>
-      <c r="I8" s="217"/>
-      <c r="J8" s="217"/>
-      <c r="K8" s="217"/>
-      <c r="L8" s="217"/>
-      <c r="M8" s="218"/>
+      <c r="E8" s="210"/>
+      <c r="F8" s="211"/>
+      <c r="G8" s="211"/>
+      <c r="H8" s="217"/>
+      <c r="I8" s="218"/>
+      <c r="J8" s="218"/>
+      <c r="K8" s="218"/>
+      <c r="L8" s="218"/>
+      <c r="M8" s="219"/>
     </row>
     <row r="9" spans="1:13" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
@@ -5030,15 +5033,15 @@
       <c r="C9" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="209"/>
-      <c r="F9" s="210"/>
-      <c r="G9" s="210"/>
-      <c r="H9" s="216"/>
-      <c r="I9" s="217"/>
-      <c r="J9" s="217"/>
-      <c r="K9" s="217"/>
-      <c r="L9" s="217"/>
-      <c r="M9" s="218"/>
+      <c r="E9" s="210"/>
+      <c r="F9" s="211"/>
+      <c r="G9" s="211"/>
+      <c r="H9" s="217"/>
+      <c r="I9" s="218"/>
+      <c r="J9" s="218"/>
+      <c r="K9" s="218"/>
+      <c r="L9" s="218"/>
+      <c r="M9" s="219"/>
     </row>
     <row r="10" spans="1:13" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
@@ -5050,15 +5053,15 @@
       <c r="C10" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="209"/>
-      <c r="F10" s="210"/>
-      <c r="G10" s="210"/>
-      <c r="H10" s="216"/>
-      <c r="I10" s="217"/>
-      <c r="J10" s="217"/>
-      <c r="K10" s="217"/>
-      <c r="L10" s="217"/>
-      <c r="M10" s="218"/>
+      <c r="E10" s="210"/>
+      <c r="F10" s="211"/>
+      <c r="G10" s="211"/>
+      <c r="H10" s="217"/>
+      <c r="I10" s="218"/>
+      <c r="J10" s="218"/>
+      <c r="K10" s="218"/>
+      <c r="L10" s="218"/>
+      <c r="M10" s="219"/>
     </row>
     <row r="11" spans="1:13" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
@@ -5070,15 +5073,15 @@
       <c r="C11" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="209"/>
-      <c r="F11" s="210"/>
-      <c r="G11" s="210"/>
-      <c r="H11" s="216"/>
-      <c r="I11" s="217"/>
-      <c r="J11" s="217"/>
-      <c r="K11" s="217"/>
-      <c r="L11" s="217"/>
-      <c r="M11" s="218"/>
+      <c r="E11" s="210"/>
+      <c r="F11" s="211"/>
+      <c r="G11" s="211"/>
+      <c r="H11" s="217"/>
+      <c r="I11" s="218"/>
+      <c r="J11" s="218"/>
+      <c r="K11" s="218"/>
+      <c r="L11" s="218"/>
+      <c r="M11" s="219"/>
     </row>
     <row r="12" spans="1:13" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
@@ -5090,15 +5093,15 @@
       <c r="C12" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="209"/>
-      <c r="F12" s="210"/>
-      <c r="G12" s="210"/>
-      <c r="H12" s="216"/>
-      <c r="I12" s="217"/>
-      <c r="J12" s="217"/>
-      <c r="K12" s="217"/>
-      <c r="L12" s="217"/>
-      <c r="M12" s="218"/>
+      <c r="E12" s="210"/>
+      <c r="F12" s="211"/>
+      <c r="G12" s="211"/>
+      <c r="H12" s="217"/>
+      <c r="I12" s="218"/>
+      <c r="J12" s="218"/>
+      <c r="K12" s="218"/>
+      <c r="L12" s="218"/>
+      <c r="M12" s="219"/>
     </row>
     <row r="13" spans="1:13" ht="34.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
@@ -5110,35 +5113,35 @@
       <c r="C13" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="211"/>
-      <c r="F13" s="212"/>
-      <c r="G13" s="212"/>
-      <c r="H13" s="219"/>
-      <c r="I13" s="220"/>
-      <c r="J13" s="220"/>
-      <c r="K13" s="220"/>
-      <c r="L13" s="220"/>
-      <c r="M13" s="221"/>
+      <c r="E13" s="212"/>
+      <c r="F13" s="213"/>
+      <c r="G13" s="213"/>
+      <c r="H13" s="220"/>
+      <c r="I13" s="221"/>
+      <c r="J13" s="221"/>
+      <c r="K13" s="221"/>
+      <c r="L13" s="221"/>
+      <c r="M13" s="222"/>
     </row>
     <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A15" s="200" t="s">
+      <c r="A15" s="201" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="201"/>
-      <c r="C15" s="201"/>
-      <c r="D15" s="201"/>
-      <c r="E15" s="202"/>
+      <c r="B15" s="202"/>
+      <c r="C15" s="202"/>
+      <c r="D15" s="202"/>
+      <c r="E15" s="203"/>
       <c r="F15" s="15"/>
-      <c r="G15" s="200" t="s">
+      <c r="G15" s="201" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="201"/>
-      <c r="I15" s="201"/>
-      <c r="J15" s="201"/>
-      <c r="K15" s="201"/>
-      <c r="L15" s="201"/>
-      <c r="M15" s="202"/>
+      <c r="H15" s="202"/>
+      <c r="I15" s="202"/>
+      <c r="J15" s="202"/>
+      <c r="K15" s="202"/>
+      <c r="L15" s="202"/>
+      <c r="M15" s="203"/>
     </row>
     <row r="16" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
@@ -5159,31 +5162,31 @@
       <c r="A17" s="123" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="203" t="s">
+      <c r="B17" s="204" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="203"/>
-      <c r="D17" s="203"/>
-      <c r="E17" s="204"/>
+      <c r="C17" s="204"/>
+      <c r="D17" s="204"/>
+      <c r="E17" s="205"/>
       <c r="F17" s="108"/>
       <c r="G17" s="123" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="198" t="s">
+      <c r="H17" s="199" t="s">
         <v>242</v>
       </c>
-      <c r="I17" s="198"/>
-      <c r="J17" s="198"/>
-      <c r="K17" s="198"/>
-      <c r="L17" s="198"/>
-      <c r="M17" s="199"/>
+      <c r="I17" s="199"/>
+      <c r="J17" s="199"/>
+      <c r="K17" s="199"/>
+      <c r="L17" s="199"/>
+      <c r="M17" s="200"/>
     </row>
     <row r="18" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="124"/>
-      <c r="B18" s="203"/>
-      <c r="C18" s="203"/>
-      <c r="D18" s="203"/>
-      <c r="E18" s="204"/>
+      <c r="B18" s="204"/>
+      <c r="C18" s="204"/>
+      <c r="D18" s="204"/>
+      <c r="E18" s="205"/>
       <c r="F18" s="108"/>
       <c r="G18" s="125"/>
       <c r="H18" s="3"/>
@@ -5197,10 +5200,10 @@
       <c r="A19" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="205"/>
-      <c r="C19" s="205"/>
-      <c r="D19" s="205"/>
-      <c r="E19" s="206"/>
+      <c r="B19" s="206"/>
+      <c r="C19" s="206"/>
+      <c r="D19" s="206"/>
+      <c r="E19" s="207"/>
       <c r="F19" s="108"/>
       <c r="G19" s="127" t="s">
         <v>241</v>
@@ -7067,8 +7070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView topLeftCell="B7" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -7076,8 +7079,8 @@
     <col min="1" max="1" width="21.44140625" style="41" customWidth="1"/>
     <col min="2" max="2" width="51.77734375" style="41" customWidth="1"/>
     <col min="3" max="3" width="55.109375" style="41" customWidth="1"/>
-    <col min="4" max="4" width="38.77734375" style="41" customWidth="1"/>
-    <col min="5" max="5" width="40.44140625" style="41" customWidth="1"/>
+    <col min="4" max="4" width="71.5546875" style="41" customWidth="1"/>
+    <col min="5" max="5" width="70.33203125" style="41" customWidth="1"/>
     <col min="6" max="6" width="15.88671875" style="107" customWidth="1"/>
     <col min="7" max="7" width="27.6640625" style="107" customWidth="1"/>
     <col min="8" max="10" width="12.109375" style="107" customWidth="1"/>
@@ -7182,7 +7185,7 @@
       <c r="A4" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="B4" s="225" t="s">
+      <c r="B4" s="136" t="s">
         <v>149</v>
       </c>
       <c r="C4" s="42" t="s">
@@ -7406,7 +7409,7 @@
       <c r="A11" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="B11" s="225" t="s">
+      <c r="B11" s="136" t="s">
         <v>164</v>
       </c>
       <c r="C11" s="42" t="s">
@@ -7470,7 +7473,7 @@
       <c r="A13" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="B13" s="225" t="s">
+      <c r="B13" s="136" t="s">
         <v>167</v>
       </c>
       <c r="C13" s="42" t="s">
@@ -7534,7 +7537,7 @@
       <c r="A15" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="B15" s="225" t="s">
+      <c r="B15" s="136" t="s">
         <v>170</v>
       </c>
       <c r="C15" s="42" t="s">
@@ -7598,7 +7601,7 @@
       <c r="A17" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="225" t="s">
+      <c r="B17" s="136" t="s">
         <v>174</v>
       </c>
       <c r="C17" s="42" t="s">
@@ -7694,7 +7697,7 @@
       <c r="A20" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="B20" s="225" t="s">
+      <c r="B20" s="136" t="s">
         <v>181</v>
       </c>
       <c r="C20" s="42" t="s">
@@ -7790,7 +7793,7 @@
       <c r="A23" s="128" t="s">
         <v>106</v>
       </c>
-      <c r="B23" s="225" t="s">
+      <c r="B23" s="136" t="s">
         <v>187</v>
       </c>
       <c r="C23" s="128" t="s">
@@ -8165,8 +8168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.6640625" defaultRowHeight="15.45" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>